<commit_message>
Dernière version du journal de bord
</commit_message>
<xml_diff>
--- a/Documentation/Tableau_de_bord.xlsx
+++ b/Documentation/Tableau_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -66,6 +66,20 @@
   </si>
   <si>
     <t>4 périodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avancer dans la partie connexion/inscription du site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 période </t>
+  </si>
+  <si>
+    <t>Entretien avec M. Egger pour faire un point sur ma documentation, je dois faire des modifications dans ma planification, améliorer mon MLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification du MLD, j'ai ajouté une table pour le paiement des articles,
+j'ai aussi enlevé deux tables et ajouté deux nouveaux champs, dans la table article, qui sont 
+taille et couleur </t>
   </si>
 </sst>
 </file>
@@ -101,9 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +522,39 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43140</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43140</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43140</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout des choses dans les docs
</commit_message>
<xml_diff>
--- a/Documentation/Tableau_de_bord.xlsx
+++ b/Documentation/Tableau_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -77,9 +77,23 @@
     <t>Entretien avec M. Egger pour faire un point sur ma documentation, je dois faire des modifications dans ma planification, améliorer mon MLD</t>
   </si>
   <si>
-    <t xml:space="preserve">Modification du MLD, j'ai ajouté une table pour le paiement des articles,
-j'ai aussi enlevé deux tables et ajouté deux nouveaux champs, dans la table article, qui sont 
-taille et couleur </t>
+    <t>Modification du MLD, j'ai ajouté une table pour le paiement des articles, j'ai décidé de laissé la table taille et couleur dans mon MLD</t>
+  </si>
+  <si>
+    <t>1er semaine</t>
+  </si>
+  <si>
+    <t>2ème semaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3ème semaine </t>
+  </si>
+  <si>
+    <t>J'ai modifié ma base de donnée en ajoutant un nouveau champ dans la table article.
+J'ai ajouté des choses dans mes use case, j'ai aussi modifié plusieurs pages du site internet pour que les liens entre les pages soient justes. J'ai supprimé des blocs du site que je n'allais pas utiliser. Ajout d'une nouvelle table dans mon MLD</t>
+  </si>
+  <si>
+    <t>6 périodes</t>
   </si>
 </sst>
 </file>
@@ -95,12 +109,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,11 +135,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,25 +439,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>43132</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43132</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -439,7 +461,7 @@
         <v>43132</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -447,32 +469,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43133</v>
+        <v>43132</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>43133</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43133</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -480,82 +494,144 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43137</v>
+        <v>43133</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43137</v>
+        <v>43133</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>43138</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43139</v>
+        <v>43137</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <v>43137</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43138</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43139</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>43140</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>43140</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>43140</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C19" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43144</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A20:C20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Journal de bord mis à jour
</commit_message>
<xml_diff>
--- a/Documentation/Tableau_de_bord.xlsx
+++ b/Documentation/Tableau_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -94,6 +94,10 @@
   </si>
   <si>
     <t>6 périodes</t>
+  </si>
+  <si>
+    <t>J'ai modifié la base de données en ajoutant un champs pour les illustrations des chaussures, 
+j'ai ajouté des données pour que dans la page de shopping il y ait des chaussures qui s'affichent. J'ai réglé un problème que j'avais lorsque je m'inscrivais sur le site, il y avait une erreur PhP qui disait qu'il ne connaissait pas des variables.</t>
   </si>
 </sst>
 </file>
@@ -427,15 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="82.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,6 +628,17 @@
       </c>
       <c r="C21" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43145</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remplissage du journal de bord
</commit_message>
<xml_diff>
--- a/Documentation/Tableau_de_bord.xlsx
+++ b/Documentation/Tableau_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -98,6 +98,12 @@
   <si>
     <t>J'ai modifié la base de données en ajoutant un champs pour les illustrations des chaussures, 
 j'ai ajouté des données pour que dans la page de shopping il y ait des chaussures qui s'affichent. J'ai réglé un problème que j'avais lorsque je m'inscrivais sur le site, il y avait une erreur PhP qui disait qu'il ne connaissait pas des variables.</t>
+  </si>
+  <si>
+    <t>J'ai listé les articles dans la page product.php. Tous les articles que j'ai dans ma base de données sont affichés dans cette page. J'ai aussi mis un filtre sur les articles pour avoir le choix d'afficher uniquement des habits, des chaussures ou seulement les sacs à dos, mais j'eu eu un souci avec cette fonction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai rélgé mon problème de fonction que j'avais la veille. Il est maintenant possible d'appliquer les filtres sur les types d'articles que l'on souhaite. </t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +647,28 @@
         <v>6</v>
       </c>
     </row>
+    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43146</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43147</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
Ajout des nouvelles activités
</commit_message>
<xml_diff>
--- a/Documentation/Tableau_de_bord.xlsx
+++ b/Documentation/Tableau_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -104,6 +104,16 @@
   </si>
   <si>
     <t xml:space="preserve">J'ai rélgé mon problème de fonction que j'avais la veille. Il est maintenant possible d'appliquer les filtres sur les types d'articles que l'on souhaite. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4ème semaine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changement à faire dans la base de données suite au nouveau cahier des charges qui m'a été envoyé par M. Carrel. J'ai enlevé des champs que je n'utiliserai pas. J'ai aussi ajouté de nouveaux uses cases. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai commencé à attaquer la partie administration pour l'administrateur du site. 
+J'ai affiché tous mes articles avec une illustration, le nom, le prix, la quantité et deux boutons pour modifier et supprimer. Quand on clique sur modifier un autre bouton apparait pour appliquer notre changement </t>
   </si>
 </sst>
 </file>
@@ -437,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,11 +679,41 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>42793</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43158</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rédaction du journal de bord
J'ai ajouté mes activités du jour
</commit_message>
<xml_diff>
--- a/Documentation/Tableau_de_bord.xlsx
+++ b/Documentation/Tableau_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -114,6 +114,9 @@
   <si>
     <t xml:space="preserve">J'ai commencé à attaquer la partie administration pour l'administrateur du site. 
 J'ai affiché tous mes articles avec une illustration, le nom, le prix, la quantité et deux boutons pour modifier et supprimer. Quand on clique sur modifier un autre bouton apparait pour appliquer notre changement </t>
+  </si>
+  <si>
+    <t>J'ai fini la fonction qui permait de modifier et supprimer un article de la base de données. Je suis en train de commencer à faire celle pour ajouter un nouvel article dans la base de données. J'ai ajouté aussi des choses dans la documentation du projet dans la partie planification et celle pour le MLD</t>
   </si>
 </sst>
 </file>
@@ -447,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,6 +711,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43159</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
Création de la fonction pour ajouter des nouveaux articles
</commit_message>
<xml_diff>
--- a/Documentation/Tableau_de_bord.xlsx
+++ b/Documentation/Tableau_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>J'ai fini la fonction qui permait de modifier et supprimer un article de la base de données. Je suis en train de commencer à faire celle pour ajouter un nouvel article dans la base de données. J'ai ajouté aussi des choses dans la documentation du projet dans la partie planification et celle pour le MLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction de la documentation du projet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai commencé la fonction qui me permettra d'ajouter des nouveaux articles dans la base de données </t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +728,28 @@
         <v>6</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43160</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43160</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>

</xml_diff>